<commit_message>
element_isenabled,element_isdisabled are included in the list.
</commit_message>
<xml_diff>
--- a/Fulcrum_FluidTX_Trunk/src/com/proj/objectRepository/ObjectsFile_Documents.xlsx
+++ b/Fulcrum_FluidTX_Trunk/src/com/proj/objectRepository/ObjectsFile_Documents.xlsx
@@ -5,7 +5,7 @@
   <workbookPr updateLinks="always"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GIWS\Falcrum_Trunk\src\com\proj\objectRepository\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GITWS_Fluid_Sprint1\Fulcrum_FluidTX_Trunk\src\com\proj\objectRepository\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="63">
   <si>
     <t>textbox</t>
   </si>
@@ -199,6 +199,21 @@
   </si>
   <si>
     <t>.//*[contains(@id,'Title_')]</t>
+  </si>
+  <si>
+    <t>selectitembytextfromlist</t>
+  </si>
+  <si>
+    <t>element_enable</t>
+  </si>
+  <si>
+    <t>element_disable</t>
+  </si>
+  <si>
+    <t>element_displayed</t>
+  </si>
+  <si>
+    <t>element_notdisplayed</t>
   </si>
 </sst>
 </file>
@@ -633,10 +648,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:A32"/>
+  <dimension ref="A2:A37"/>
   <sheetViews>
     <sheetView topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="B32" sqref="B32"/>
+      <selection activeCell="A36" sqref="A36:A37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -797,6 +812,31 @@
     <row r="32" spans="1:1">
       <c r="A32" t="s">
         <v>43</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1">
+      <c r="A33" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1">
+      <c r="A34" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1">
+      <c r="A35" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1">
+      <c r="A36" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1">
+      <c r="A37" t="s">
+        <v>62</v>
       </c>
     </row>
   </sheetData>

</xml_diff>